<commit_message>
2018年 12月 29日 星期六 17:17:20 +08
</commit_message>
<xml_diff>
--- a/Protocol_Analysis/lists/Function_list.xlsx
+++ b/Protocol_Analysis/lists/Function_list.xlsx
@@ -129,9 +129,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -163,10 +163,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -187,6 +188,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -210,15 +218,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,7 +280,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,44 +288,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,25 +302,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,157 +368,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,18 +509,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,9 +570,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -578,141 +593,126 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -724,19 +724,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
2018年 12月 30日 星期日 16:06:37 +08
</commit_message>
<xml_diff>
--- a/Protocol_Analysis/lists/Function_list.xlsx
+++ b/Protocol_Analysis/lists/Function_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="162">
   <si>
     <t>核心功能</t>
   </si>
@@ -190,6 +190,27 @@
     <t>crit_addr</t>
   </si>
   <si>
+    <t>send-buf.h</t>
+  </si>
+  <si>
+    <t>crit_garbage</t>
+  </si>
+  <si>
+    <t>crit_addr_id_del</t>
+  </si>
+  <si>
+    <t>maint-buf.h</t>
+  </si>
+  <si>
+    <t>crit_addr_del</t>
+  </si>
+  <si>
+    <t>crit_ack_req_sent</t>
+  </si>
+  <si>
+    <t>crit_expires</t>
+  </si>
+  <si>
     <t>crit_duplicate</t>
   </si>
   <si>
@@ -377,6 +398,108 @@
   </si>
   <si>
     <t>tbl_for_each_del</t>
+  </si>
+  <si>
+    <t>send_buf_print</t>
+  </si>
+  <si>
+    <t>send-buf基本操作</t>
+  </si>
+  <si>
+    <t>send_buf_set_max_len</t>
+  </si>
+  <si>
+    <t>send_buf_timeout</t>
+  </si>
+  <si>
+    <t>send_buf_entry_create</t>
+  </si>
+  <si>
+    <t>send_buf_enqueue_packet</t>
+  </si>
+  <si>
+    <t>send_buf_set_verdict</t>
+  </si>
+  <si>
+    <t>send_buf_flush</t>
+  </si>
+  <si>
+    <t>send_buf_get_info</t>
+  </si>
+  <si>
+    <t>send_buf_cleanup</t>
+  </si>
+  <si>
+    <t>maint_buf_init</t>
+  </si>
+  <si>
+    <t>maint-buf基本操作</t>
+  </si>
+  <si>
+    <t>maint_buf_cleanup</t>
+  </si>
+  <si>
+    <t>maint_buf_set_max_len</t>
+  </si>
+  <si>
+    <t>maint_buf_add</t>
+  </si>
+  <si>
+    <t>maint_buf_del_all</t>
+  </si>
+  <si>
+    <t>maint_buf_del_all_id</t>
+  </si>
+  <si>
+    <t>maint_buf_del_addr</t>
+  </si>
+  <si>
+    <t>maint_buf_set_timeout</t>
+  </si>
+  <si>
+    <t>maint_buf_timeout</t>
+  </si>
+  <si>
+    <t>maint_buf_salvage</t>
+  </si>
+  <si>
+    <t>lc_link_del</t>
+  </si>
+  <si>
+    <t>link-cache基本操作</t>
+  </si>
+  <si>
+    <t>link-cache.h</t>
+  </si>
+  <si>
+    <t>lc_link_add</t>
+  </si>
+  <si>
+    <t>lc_garbage_collect_set</t>
+  </si>
+  <si>
+    <t>lc_garbage_collect</t>
+  </si>
+  <si>
+    <t>lc_srt_find</t>
+  </si>
+  <si>
+    <t>lc_srt_add</t>
+  </si>
+  <si>
+    <t>lc_flush</t>
+  </si>
+  <si>
+    <t>lc_init</t>
+  </si>
+  <si>
+    <t>lc_cleanup</t>
+  </si>
+  <si>
+    <t>__dijkstra</t>
+  </si>
+  <si>
+    <t>迪杰斯特拉运算</t>
   </si>
 </sst>
 </file>
@@ -384,10 +507,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -404,8 +527,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -420,12 +573,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -435,22 +597,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,21 +628,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,59 +656,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -557,103 +680,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,84 +836,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -803,6 +926,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -814,6 +968,56 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -841,216 +1045,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1075,17 +1220,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1406,10 +1569,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89:C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
@@ -1499,7 +1662,7 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1511,7 +1674,7 @@
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1523,7 +1686,7 @@
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1535,7 +1698,7 @@
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1547,7 +1710,7 @@
       <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1559,7 +1722,7 @@
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1567,22 +1730,22 @@
       </c>
     </row>
     <row r="14" spans="4:4">
-      <c r="D14" s="9"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="4:4">
-      <c r="D15" s="9"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="4:4">
-      <c r="D16" s="9"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="4:4">
-      <c r="D17" s="9"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="22" spans="4:4">
-      <c r="D22" s="10"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="4:4">
-      <c r="D23" s="10"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
@@ -1599,8 +1762,8 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1611,8 +1774,8 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1621,8 +1784,8 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="2"/>
-      <c r="B27" s="11" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1631,8 +1794,8 @@
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="2"/>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1641,8 +1804,8 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="2"/>
-      <c r="B29" s="1" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1651,8 +1814,8 @@
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="2"/>
-      <c r="B30" s="1" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1663,8 +1826,8 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="2"/>
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1673,8 +1836,8 @@
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="2"/>
-      <c r="B32" s="1" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1683,8 +1846,8 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="2"/>
-      <c r="B33" s="1" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1693,8 +1856,8 @@
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="2"/>
-      <c r="B34" s="1" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1703,8 +1866,8 @@
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="1" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1715,8 +1878,8 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1727,432 +1890,734 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="2"/>
-      <c r="B37" s="1" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="2"/>
-      <c r="B38" s="1" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="11" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="9"/>
+      <c r="B39" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="9"/>
+      <c r="B40" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="9"/>
+      <c r="B41" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="9"/>
+      <c r="B42" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="9"/>
+      <c r="B43" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="15"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="9"/>
+      <c r="B44" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="14"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="9"/>
+      <c r="B45" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2"/>
-      <c r="B39" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="2"/>
-      <c r="B40" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="2" t="s">
+    <row r="46" spans="1:4">
+      <c r="A46" s="9"/>
+      <c r="B46" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="9"/>
+      <c r="B47" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2"/>
-      <c r="B41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="2"/>
-      <c r="B42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2"/>
-      <c r="B43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2"/>
-      <c r="B44" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2"/>
-      <c r="B45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2"/>
-      <c r="B46" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="2"/>
-      <c r="B47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="1" t="s">
+    <row r="48" spans="1:4">
+      <c r="A48" s="9"/>
+      <c r="B48" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="9"/>
+      <c r="B49" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="9"/>
+      <c r="B50" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="9"/>
+      <c r="B51" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="9"/>
+      <c r="B52" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="9"/>
+      <c r="B53" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="9"/>
+      <c r="B54" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="2"/>
-      <c r="B48" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" s="2" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" s="9"/>
+      <c r="B55" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="2"/>
-      <c r="B49" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2"/>
-      <c r="B50" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2"/>
-      <c r="B51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2"/>
-      <c r="B52" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" s="2" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" s="9"/>
+      <c r="B56" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="2"/>
-      <c r="B53" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="9"/>
+      <c r="B57" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="2"/>
-      <c r="B54" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="9"/>
+      <c r="B58" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="2"/>
-      <c r="B55" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="9"/>
+      <c r="B59" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="2"/>
-      <c r="B56" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="9"/>
+      <c r="B60" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="C60" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="9"/>
+      <c r="B61" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="9"/>
+      <c r="B62" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="9"/>
+      <c r="B63" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="2"/>
-      <c r="B57" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="2"/>
-      <c r="B58" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="2"/>
-      <c r="B59" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="2"/>
-      <c r="B60" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="2" t="s">
+    <row r="64" spans="1:4">
+      <c r="A64" s="9"/>
+      <c r="B64" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="2"/>
-      <c r="B61" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="9"/>
+      <c r="B65" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="2"/>
-      <c r="B62" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="9"/>
+      <c r="B66" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="2"/>
-      <c r="B63" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="9"/>
+      <c r="B67" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="2"/>
-      <c r="B64" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="9"/>
+      <c r="B68" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="2"/>
-      <c r="B65" s="1" t="s">
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="9"/>
+      <c r="B69" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="2"/>
-      <c r="B66" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="2"/>
-      <c r="B67" s="1" t="s">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="9"/>
+      <c r="B70" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2"/>
-      <c r="B68" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="2"/>
-      <c r="B69" s="1" t="s">
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="9"/>
+      <c r="B71" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="2"/>
-      <c r="B70" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="2"/>
-      <c r="B71" s="1" t="s">
+      <c r="D71" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="2"/>
-      <c r="B72" s="1" t="s">
+      <c r="A72" s="9"/>
+      <c r="B72" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="2"/>
-      <c r="B73" s="1" t="s">
+      <c r="A73" s="9"/>
+      <c r="B73" s="11" t="s">
         <v>112</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="2"/>
-      <c r="B74" s="1" t="s">
+      <c r="A74" s="9"/>
+      <c r="B74" s="11" t="s">
         <v>113</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="2"/>
-      <c r="B75" s="1" t="s">
+      <c r="A75" s="9"/>
+      <c r="B75" s="11" t="s">
         <v>114</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="2"/>
-      <c r="B76" s="1" t="s">
+      <c r="A76" s="9"/>
+      <c r="B76" s="11" t="s">
         <v>115</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="2"/>
-      <c r="B77" s="1" t="s">
+      <c r="A77" s="9"/>
+      <c r="B77" s="11" t="s">
         <v>116</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="2"/>
-      <c r="B78" s="1" t="s">
+      <c r="A78" s="9"/>
+      <c r="B78" s="11" t="s">
         <v>117</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="2"/>
-      <c r="B79" s="1" t="s">
+      <c r="A79" s="9"/>
+      <c r="B79" s="11" t="s">
         <v>118</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="2"/>
-      <c r="B80" s="1" t="s">
+      <c r="A80" s="9"/>
+      <c r="B80" s="11" t="s">
         <v>119</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="2"/>
-      <c r="B81" s="1" t="s">
+      <c r="A81" s="9"/>
+      <c r="B81" s="11" t="s">
         <v>120</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="9"/>
+      <c r="B82" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="9"/>
+      <c r="B83" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="9"/>
+      <c r="B84" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="9"/>
+      <c r="B85" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="9"/>
+      <c r="B86" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="9"/>
+      <c r="B87" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="9"/>
+      <c r="B88" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="9"/>
+      <c r="B89" t="s">
+        <v>128</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="9"/>
+      <c r="B90" t="s">
+        <v>130</v>
+      </c>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="9"/>
+      <c r="B91" t="s">
+        <v>131</v>
+      </c>
+      <c r="C91" s="16"/>
+      <c r="D91" s="16"/>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="9"/>
+      <c r="B92" t="s">
+        <v>132</v>
+      </c>
+      <c r="C92" s="16"/>
+      <c r="D92" s="16"/>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="9"/>
+      <c r="B93" t="s">
+        <v>133</v>
+      </c>
+      <c r="C93" s="16"/>
+      <c r="D93" s="16"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="9"/>
+      <c r="B94" t="s">
+        <v>134</v>
+      </c>
+      <c r="C94" s="16"/>
+      <c r="D94" s="16"/>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="9"/>
+      <c r="B95" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95" s="16"/>
+      <c r="D95" s="16"/>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="9"/>
+      <c r="B96" t="s">
+        <v>128</v>
+      </c>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="9"/>
+      <c r="B97" t="s">
+        <v>136</v>
+      </c>
+      <c r="C97" s="16"/>
+      <c r="D97" s="16"/>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="9"/>
+      <c r="B98" t="s">
+        <v>137</v>
+      </c>
+      <c r="C98" s="16"/>
+      <c r="D98" s="16"/>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" t="s">
+        <v>138</v>
+      </c>
+      <c r="C99" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="B100" t="s">
+        <v>140</v>
+      </c>
+      <c r="C100" s="16"/>
+      <c r="D100" s="16"/>
+    </row>
+    <row r="101" spans="2:4">
+      <c r="B101" t="s">
+        <v>141</v>
+      </c>
+      <c r="C101" s="16"/>
+      <c r="D101" s="16"/>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102" t="s">
+        <v>142</v>
+      </c>
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
+    </row>
+    <row r="103" spans="2:4">
+      <c r="B103" t="s">
+        <v>143</v>
+      </c>
+      <c r="C103" s="16"/>
+      <c r="D103" s="16"/>
+    </row>
+    <row r="104" spans="2:4">
+      <c r="B104" t="s">
+        <v>144</v>
+      </c>
+      <c r="C104" s="16"/>
+      <c r="D104" s="16"/>
+    </row>
+    <row r="105" spans="2:4">
+      <c r="B105" t="s">
+        <v>145</v>
+      </c>
+      <c r="C105" s="16"/>
+      <c r="D105" s="16"/>
+    </row>
+    <row r="106" spans="2:4">
+      <c r="B106" t="s">
+        <v>146</v>
+      </c>
+      <c r="C106" s="16"/>
+      <c r="D106" s="16"/>
+    </row>
+    <row r="107" spans="2:4">
+      <c r="B107" t="s">
+        <v>147</v>
+      </c>
+      <c r="C107" s="16"/>
+      <c r="D107" s="16"/>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" t="s">
+        <v>148</v>
+      </c>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
+    </row>
+    <row r="109" spans="2:4">
+      <c r="B109" t="s">
+        <v>149</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110" t="s">
+        <v>152</v>
+      </c>
+      <c r="C110" s="16"/>
+      <c r="D110" s="16"/>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="B111" t="s">
+        <v>153</v>
+      </c>
+      <c r="C111" s="16"/>
+      <c r="D111" s="16"/>
+    </row>
+    <row r="112" spans="2:4">
+      <c r="B112" t="s">
+        <v>154</v>
+      </c>
+      <c r="C112" s="16"/>
+      <c r="D112" s="16"/>
+    </row>
+    <row r="113" spans="2:4">
+      <c r="B113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C113" s="16"/>
+      <c r="D113" s="16"/>
+    </row>
+    <row r="114" spans="2:4">
+      <c r="B114" t="s">
+        <v>156</v>
+      </c>
+      <c r="C114" s="16"/>
+      <c r="D114" s="16"/>
+    </row>
+    <row r="115" spans="2:4">
+      <c r="B115" t="s">
+        <v>157</v>
+      </c>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
+    </row>
+    <row r="116" spans="2:4">
+      <c r="B116" t="s">
+        <v>158</v>
+      </c>
+      <c r="C116" s="16"/>
+      <c r="D116" s="16"/>
+    </row>
+    <row r="117" spans="2:4">
+      <c r="B117" t="s">
+        <v>159</v>
+      </c>
+      <c r="C117" s="16"/>
+      <c r="D117" s="16"/>
+    </row>
+    <row r="118" spans="2:4">
+      <c r="B118" t="s">
+        <v>160</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D118" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="23">
     <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A25:A81"/>
+    <mergeCell ref="A25:A98"/>
     <mergeCell ref="C2:C7"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C46"/>
-    <mergeCell ref="C64:C81"/>
+    <mergeCell ref="C36:C46"/>
+    <mergeCell ref="C47:C53"/>
+    <mergeCell ref="C71:C88"/>
+    <mergeCell ref="C89:C98"/>
+    <mergeCell ref="C99:C108"/>
+    <mergeCell ref="C109:C117"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D25:D29"/>
     <mergeCell ref="D30:D34"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D46"/>
-    <mergeCell ref="D48:D55"/>
-    <mergeCell ref="D56:D63"/>
-    <mergeCell ref="D64:D81"/>
+    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D47:D53"/>
+    <mergeCell ref="D55:D62"/>
+    <mergeCell ref="D63:D70"/>
+    <mergeCell ref="D71:D88"/>
+    <mergeCell ref="D89:D98"/>
+    <mergeCell ref="D99:D108"/>
+    <mergeCell ref="D109:D118"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
2018年 12月 30日 星期日 16:06:59 +08
</commit_message>
<xml_diff>
--- a/Protocol_Analysis/lists/Function_list.xlsx
+++ b/Protocol_Analysis/lists/Function_list.xlsx
@@ -865,7 +865,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -920,28 +920,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1059,7 +1037,7 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1092,7 +1070,7 @@
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1110,19 +1088,19 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1158,7 +1136,7 @@
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1176,13 +1154,13 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1191,11 +1169,11 @@
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1226,28 +1204,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1571,8 +1537,8 @@
   <sheetPr/>
   <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89:C98"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A110" sqref="A24:D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
@@ -1763,7 +1729,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="10"/>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1774,8 +1740,8 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="11" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1784,8 +1750,8 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="12" t="s">
+      <c r="A27" s="10"/>
+      <c r="B27" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1794,8 +1760,8 @@
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="11" t="s">
+      <c r="A28" s="10"/>
+      <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1804,8 +1770,8 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="9"/>
-      <c r="B29" s="11" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1814,8 +1780,8 @@
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="9"/>
-      <c r="B30" s="11" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1826,8 +1792,8 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="9"/>
-      <c r="B31" s="11" t="s">
+      <c r="A31" s="10"/>
+      <c r="B31" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1836,8 +1802,8 @@
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="9"/>
-      <c r="B32" s="11" t="s">
+      <c r="A32" s="10"/>
+      <c r="B32" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1846,8 +1812,8 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="9"/>
-      <c r="B33" s="11" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1856,8 +1822,8 @@
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="9"/>
-      <c r="B34" s="11" t="s">
+      <c r="A34" s="10"/>
+      <c r="B34" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1866,8 +1832,8 @@
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="11" t="s">
+      <c r="A35" s="10"/>
+      <c r="B35" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1878,8 +1844,8 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="9"/>
-      <c r="B36" s="11" t="s">
+      <c r="A36" s="10"/>
+      <c r="B36" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1890,76 +1856,76 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="9"/>
-      <c r="B37" s="11" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="9"/>
-      <c r="B38" s="11" t="s">
+      <c r="A38" s="10"/>
+      <c r="B38" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="9"/>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="10"/>
+      <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C39" s="2"/>
-      <c r="D39" s="14"/>
+      <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="9"/>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="10"/>
+      <c r="B40" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="9"/>
-      <c r="B41" s="11" t="s">
+      <c r="A41" s="10"/>
+      <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="15"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="9"/>
-      <c r="B42" s="11" t="s">
+      <c r="A42" s="10"/>
+      <c r="B42" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="15"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="9"/>
-      <c r="B43" s="11" t="s">
+      <c r="A43" s="10"/>
+      <c r="B43" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="15"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="9"/>
-      <c r="B44" s="11" t="s">
+      <c r="A44" s="10"/>
+      <c r="B44" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="14"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="9"/>
-      <c r="B45" s="11" t="s">
+      <c r="A45" s="10"/>
+      <c r="B45" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C45" s="2"/>
@@ -1968,16 +1934,16 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="9"/>
-      <c r="B46" s="11" t="s">
+      <c r="A46" s="10"/>
+      <c r="B46" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="9"/>
-      <c r="B47" s="11" t="s">
+      <c r="A47" s="10"/>
+      <c r="B47" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -1988,56 +1954,56 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="9"/>
-      <c r="B48" s="11" t="s">
+      <c r="A48" s="10"/>
+      <c r="B48" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="9"/>
-      <c r="B49" s="11" t="s">
+      <c r="A49" s="10"/>
+      <c r="B49" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="9"/>
-      <c r="B50" s="11" t="s">
+      <c r="A50" s="10"/>
+      <c r="B50" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="9"/>
-      <c r="B51" s="11" t="s">
+      <c r="A51" s="10"/>
+      <c r="B51" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="9"/>
-      <c r="B52" s="11" t="s">
+      <c r="A52" s="10"/>
+      <c r="B52" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="9"/>
-      <c r="B53" s="11" t="s">
+      <c r="A53" s="10"/>
+      <c r="B53" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="9"/>
-      <c r="B54" s="11" t="s">
+      <c r="A54" s="10"/>
+      <c r="B54" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2048,8 +2014,8 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="9"/>
-      <c r="B55" s="11" t="s">
+      <c r="A55" s="10"/>
+      <c r="B55" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -2060,8 +2026,8 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="9"/>
-      <c r="B56" s="11" t="s">
+      <c r="A56" s="10"/>
+      <c r="B56" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -2070,8 +2036,8 @@
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="9"/>
-      <c r="B57" s="11" t="s">
+      <c r="A57" s="10"/>
+      <c r="B57" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -2080,8 +2046,8 @@
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="9"/>
-      <c r="B58" s="11" t="s">
+      <c r="A58" s="10"/>
+      <c r="B58" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -2090,8 +2056,8 @@
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="9"/>
-      <c r="B59" s="11" t="s">
+      <c r="A59" s="10"/>
+      <c r="B59" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -2100,8 +2066,8 @@
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="9"/>
-      <c r="B60" s="11" t="s">
+      <c r="A60" s="10"/>
+      <c r="B60" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -2110,8 +2076,8 @@
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="9"/>
-      <c r="B61" s="11" t="s">
+      <c r="A61" s="10"/>
+      <c r="B61" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -2120,8 +2086,8 @@
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="9"/>
-      <c r="B62" s="11" t="s">
+      <c r="A62" s="10"/>
+      <c r="B62" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -2130,8 +2096,8 @@
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="9"/>
-      <c r="B63" s="11" t="s">
+      <c r="A63" s="10"/>
+      <c r="B63" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -2142,8 +2108,8 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="9"/>
-      <c r="B64" s="11" t="s">
+      <c r="A64" s="10"/>
+      <c r="B64" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -2152,8 +2118,8 @@
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="9"/>
-      <c r="B65" s="11" t="s">
+      <c r="A65" s="10"/>
+      <c r="B65" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2162,8 +2128,8 @@
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="9"/>
-      <c r="B66" s="11" t="s">
+      <c r="A66" s="10"/>
+      <c r="B66" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -2172,8 +2138,8 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="9"/>
-      <c r="B67" s="11" t="s">
+      <c r="A67" s="10"/>
+      <c r="B67" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2182,8 +2148,8 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="9"/>
-      <c r="B68" s="11" t="s">
+      <c r="A68" s="10"/>
+      <c r="B68" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -2192,8 +2158,8 @@
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="9"/>
-      <c r="B69" s="11" t="s">
+      <c r="A69" s="10"/>
+      <c r="B69" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -2202,8 +2168,8 @@
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="9"/>
-      <c r="B70" s="11" t="s">
+      <c r="A70" s="10"/>
+      <c r="B70" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -2212,8 +2178,8 @@
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="9"/>
-      <c r="B71" s="11" t="s">
+      <c r="A71" s="10"/>
+      <c r="B71" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2224,374 +2190,394 @@
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="9"/>
-      <c r="B72" s="11" t="s">
+      <c r="A72" s="10"/>
+      <c r="B72" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="9"/>
-      <c r="B73" s="11" t="s">
+      <c r="A73" s="10"/>
+      <c r="B73" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="9"/>
-      <c r="B74" s="11" t="s">
+      <c r="A74" s="10"/>
+      <c r="B74" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="9"/>
-      <c r="B75" s="11" t="s">
+      <c r="A75" s="10"/>
+      <c r="B75" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="9"/>
-      <c r="B76" s="11" t="s">
+      <c r="A76" s="10"/>
+      <c r="B76" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="9"/>
-      <c r="B77" s="11" t="s">
+      <c r="A77" s="10"/>
+      <c r="B77" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="9"/>
-      <c r="B78" s="11" t="s">
+      <c r="A78" s="10"/>
+      <c r="B78" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="9"/>
-      <c r="B79" s="11" t="s">
+      <c r="A79" s="10"/>
+      <c r="B79" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="9"/>
-      <c r="B80" s="11" t="s">
+      <c r="A80" s="10"/>
+      <c r="B80" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="9"/>
-      <c r="B81" s="11" t="s">
+      <c r="A81" s="10"/>
+      <c r="B81" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="9"/>
-      <c r="B82" s="11" t="s">
+      <c r="A82" s="10"/>
+      <c r="B82" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="9"/>
-      <c r="B83" s="11" t="s">
+      <c r="A83" s="10"/>
+      <c r="B83" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="9"/>
-      <c r="B84" s="11" t="s">
+      <c r="A84" s="10"/>
+      <c r="B84" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="9"/>
-      <c r="B85" s="11" t="s">
+      <c r="A85" s="10"/>
+      <c r="B85" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="9"/>
-      <c r="B86" s="11" t="s">
+      <c r="A86" s="10"/>
+      <c r="B86" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="9"/>
-      <c r="B87" s="11" t="s">
+      <c r="A87" s="10"/>
+      <c r="B87" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="9"/>
-      <c r="B88" s="11" t="s">
+      <c r="A88" s="10"/>
+      <c r="B88" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="9"/>
-      <c r="B89" t="s">
+      <c r="A89" s="10"/>
+      <c r="B89" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C89" s="16" t="s">
+      <c r="C89" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="9"/>
-      <c r="B90" t="s">
+      <c r="A90" s="10"/>
+      <c r="B90" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C90" s="16"/>
-      <c r="D90" s="16"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="9"/>
-      <c r="B91" t="s">
+      <c r="A91" s="10"/>
+      <c r="B91" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C91" s="16"/>
-      <c r="D91" s="16"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="9"/>
-      <c r="B92" t="s">
+      <c r="A92" s="10"/>
+      <c r="B92" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C92" s="16"/>
-      <c r="D92" s="16"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="9"/>
-      <c r="B93" t="s">
+      <c r="A93" s="10"/>
+      <c r="B93" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C93" s="16"/>
-      <c r="D93" s="16"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="9"/>
-      <c r="B94" t="s">
+      <c r="A94" s="10"/>
+      <c r="B94" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C94" s="16"/>
-      <c r="D94" s="16"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="9"/>
-      <c r="B95" t="s">
+      <c r="A95" s="10"/>
+      <c r="B95" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C95" s="16"/>
-      <c r="D95" s="16"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="9"/>
-      <c r="B96" t="s">
+      <c r="A96" s="10"/>
+      <c r="B96" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C96" s="16"/>
-      <c r="D96" s="16"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="9"/>
-      <c r="B97" t="s">
+      <c r="A97" s="10"/>
+      <c r="B97" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C97" s="16"/>
-      <c r="D97" s="16"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="9"/>
-      <c r="B98" t="s">
+      <c r="A98" s="10"/>
+      <c r="B98" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C98" s="16"/>
-      <c r="D98" s="16"/>
-    </row>
-    <row r="99" spans="2:4">
-      <c r="B99" t="s">
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="11"/>
+      <c r="B99" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C99" s="16" t="s">
+      <c r="C99" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="D99" s="16" t="s">
+      <c r="D99" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="100" spans="2:4">
-      <c r="B100" t="s">
+    <row r="100" spans="1:4">
+      <c r="A100" s="11"/>
+      <c r="B100" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C100" s="16"/>
-      <c r="D100" s="16"/>
-    </row>
-    <row r="101" spans="2:4">
-      <c r="B101" t="s">
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="11"/>
+      <c r="B101" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C101" s="16"/>
-      <c r="D101" s="16"/>
-    </row>
-    <row r="102" spans="2:4">
-      <c r="B102" t="s">
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="11"/>
+      <c r="B102" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="C102" s="16"/>
-      <c r="D102" s="16"/>
-    </row>
-    <row r="103" spans="2:4">
-      <c r="B103" t="s">
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="11"/>
+      <c r="B103" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C103" s="16"/>
-      <c r="D103" s="16"/>
-    </row>
-    <row r="104" spans="2:4">
-      <c r="B104" t="s">
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="11"/>
+      <c r="B104" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C104" s="16"/>
-      <c r="D104" s="16"/>
-    </row>
-    <row r="105" spans="2:4">
-      <c r="B105" t="s">
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C105" s="16"/>
-      <c r="D105" s="16"/>
-    </row>
-    <row r="106" spans="2:4">
-      <c r="B106" t="s">
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="11"/>
+      <c r="B106" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C106" s="16"/>
-      <c r="D106" s="16"/>
-    </row>
-    <row r="107" spans="2:4">
-      <c r="B107" t="s">
+      <c r="C106" s="12"/>
+      <c r="D106" s="12"/>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="11"/>
+      <c r="B107" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C107" s="16"/>
-      <c r="D107" s="16"/>
-    </row>
-    <row r="108" spans="2:4">
-      <c r="B108" t="s">
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="11"/>
+      <c r="B108" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C108" s="16"/>
-      <c r="D108" s="16"/>
-    </row>
-    <row r="109" spans="2:4">
-      <c r="B109" t="s">
+      <c r="C108" s="12"/>
+      <c r="D108" s="12"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="11"/>
+      <c r="B109" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C109" s="16" t="s">
+      <c r="C109" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D109" s="16" t="s">
+      <c r="D109" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="110" spans="2:4">
-      <c r="B110" t="s">
+    <row r="110" spans="1:4">
+      <c r="A110" s="11"/>
+      <c r="B110" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C110" s="16"/>
-      <c r="D110" s="16"/>
-    </row>
-    <row r="111" spans="2:4">
-      <c r="B111" t="s">
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="11"/>
+      <c r="B111" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C111" s="16"/>
-      <c r="D111" s="16"/>
-    </row>
-    <row r="112" spans="2:4">
-      <c r="B112" t="s">
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="11"/>
+      <c r="B112" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C112" s="16"/>
-      <c r="D112" s="16"/>
-    </row>
-    <row r="113" spans="2:4">
-      <c r="B113" t="s">
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="11"/>
+      <c r="B113" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C113" s="16"/>
-      <c r="D113" s="16"/>
-    </row>
-    <row r="114" spans="2:4">
-      <c r="B114" t="s">
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="11"/>
+      <c r="B114" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C114" s="16"/>
-      <c r="D114" s="16"/>
-    </row>
-    <row r="115" spans="2:4">
-      <c r="B115" t="s">
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="11"/>
+      <c r="B115" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C115" s="16"/>
-      <c r="D115" s="16"/>
-    </row>
-    <row r="116" spans="2:4">
-      <c r="B116" t="s">
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="11"/>
+      <c r="B116" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="C116" s="16"/>
-      <c r="D116" s="16"/>
-    </row>
-    <row r="117" spans="2:4">
-      <c r="B117" t="s">
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="11"/>
+      <c r="B117" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C117" s="16"/>
-      <c r="D117" s="16"/>
-    </row>
-    <row r="118" spans="2:4">
-      <c r="B118" t="s">
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="11"/>
+      <c r="B118" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C118" s="17" t="s">
+      <c r="C118" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="D118" s="16"/>
+      <c r="D118" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>